<commit_message>
Add User Acceptance Tests
</commit_message>
<xml_diff>
--- a/Documentation/Risk List/Risk List 6.1.xlsx
+++ b/Documentation/Risk List/Risk List 6.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Documents/CSU/Study/Year 3/Sem 1/Software Development 1/salesAndWarehouseSystem/Documentation/Risk List/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB672DEF-4CA8-F64B-A3D8-D34F6734507B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99799F8C-3A22-3246-BBDD-EC2D29ED0F48}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="460" windowWidth="14360" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -574,7 +574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="162">
   <si>
     <t>ID</t>
   </si>
@@ -1247,9 +1247,6 @@
     <t>The manager will have the right to give punishments to the responsible team members.</t>
   </si>
   <si>
-    <t>The database connection may be disrupted if it crosses over the limit connection.</t>
-  </si>
-  <si>
     <t>The versions of Jersey, Maven, JDK are incompetable what may cause the issues when deploying the implementation.</t>
   </si>
   <si>
@@ -1261,18 +1258,6 @@
   </si>
   <si>
     <t>The Inteillij IDEA cannot deploy the product.</t>
-  </si>
-  <si>
-    <t>Debug the product and close the connection to database every time execute a quey.</t>
-  </si>
-  <si>
-    <t>Cannot solve the bugs after the due date of task as Iteration Plan.</t>
-  </si>
-  <si>
-    <t>Ask help from other teams or the Database experts</t>
-  </si>
-  <si>
-    <t>Ask help from other teams or the IT experts</t>
   </si>
   <si>
     <t>Performance
@@ -1280,9 +1265,6 @@
 Schedule</t>
   </si>
   <si>
-    <t>The requirement is added after “freezing” the requirements.</t>
-  </si>
-  <si>
     <t>Consider the importance of this requirement or try to find other alternatives.</t>
   </si>
   <si>
@@ -1308,22 +1290,85 @@
     <t>The Error 500 will be issued.</t>
   </si>
   <si>
-    <t>Intellij cannot display the data to database when execute the product too many times.</t>
-  </si>
-  <si>
     <t>Try to find the solution through online resources or trying to delete the work.xml file.</t>
   </si>
   <si>
     <t xml:space="preserve">Try to find the solution through online resources or trying to delete and create a new artifact solved the issue. </t>
   </si>
   <si>
-    <t>Ask help from other teams or the Intellij experts</t>
-  </si>
-  <si>
     <t>Try to find the solution through online resources or trying to check the security settings of AWS.</t>
   </si>
   <si>
-    <t>Ask help from other teams or the AWS experts</t>
+    <t>System cannot carry out CRUD functions on the database .</t>
+  </si>
+  <si>
+    <t>Unable to connect to the database due to the number of request exceeding the allowed number of requests for AWS RDS.</t>
+  </si>
+  <si>
+    <t>Unable to solve the bug after the due date of task according to the  Iteration Plan.</t>
+  </si>
+  <si>
+    <t>Close the connection to database every time a connection is made.</t>
+  </si>
+  <si>
+    <t>Ask help from other developers or Database experts</t>
+  </si>
+  <si>
+    <t>Ask help from other teams or Java EE experts</t>
+  </si>
+  <si>
+    <t>Ask help from other teams or IT experts</t>
+  </si>
+  <si>
+    <t>Ask help from other teams or Java experts</t>
+  </si>
+  <si>
+    <t>Ask help from other teams or AWS experts</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>The requirement are added after “freezing” the requirements.</t>
+  </si>
+  <si>
+    <t>The requirement added to add to the system.</t>
+  </si>
+  <si>
+    <t>The Project Plan need to be extended for doing the requirements</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1378,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2242,70 +2287,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="65">
     <dxf>
       <fill>
         <patternFill>
@@ -3156,21 +3138,21 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.1640625" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="93" style="10" customWidth="1"/>
     <col min="3" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" thickBot="1">
+    <row r="1" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
       <c r="B1" s="100"/>
     </row>
-    <row r="2" spans="1:2" ht="12" thickBot="1">
+    <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="63" t="s">
         <v>12</v>
       </c>
@@ -3178,19 +3160,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="23"/>
       <c r="B3" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="20"/>
       <c r="B4" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
@@ -3198,7 +3180,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="44">
+    <row r="6" spans="1:2" ht="44" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -3206,7 +3188,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="66">
+    <row r="7" spans="1:2" ht="66" x14ac:dyDescent="0.15">
       <c r="A7" s="21" t="s">
         <v>15</v>
       </c>
@@ -3214,7 +3196,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="21" t="s">
         <v>16</v>
       </c>
@@ -3222,7 +3204,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="55">
+    <row r="9" spans="1:2" ht="55" x14ac:dyDescent="0.15">
       <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
@@ -3230,7 +3212,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="21" t="s">
         <v>18</v>
       </c>
@@ -3238,7 +3220,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="21" t="s">
         <v>19</v>
       </c>
@@ -3246,7 +3228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -3254,7 +3236,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -3262,7 +3244,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -3270,7 +3252,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -3278,7 +3260,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -3286,7 +3268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12" thickBot="1">
+    <row r="17" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
         <v>70</v>
       </c>
@@ -3294,8 +3276,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12" thickBot="1"/>
-    <row r="20" spans="1:2" ht="12" thickBot="1">
+    <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>12</v>
       </c>
@@ -3303,7 +3285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="34" thickBot="1">
+    <row r="21" spans="1:2" ht="34" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>66</v>
       </c>
@@ -3311,8 +3293,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12" thickBot="1"/>
-    <row r="24" spans="1:2" ht="12" thickBot="1">
+    <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>12</v>
       </c>
@@ -3320,7 +3302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="56" thickBot="1">
+    <row r="25" spans="1:2" ht="56" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
         <v>20</v>
       </c>
@@ -3344,11 +3326,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J11" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="J9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="6" bestFit="1" customWidth="1"/>
@@ -3365,7 +3347,7 @@
     <col min="16" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="19" thickBot="1">
+    <row r="1" spans="1:21" s="7" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -3384,7 +3366,7 @@
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -3417,7 +3399,7 @@
       <c r="T2" s="53"/>
       <c r="U2" s="53"/>
     </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1">
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>76</v>
       </c>
@@ -3450,7 +3432,7 @@
       <c r="T3" s="53"/>
       <c r="U3" s="53"/>
     </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1">
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -3483,7 +3465,7 @@
       <c r="T4" s="53"/>
       <c r="U4" s="53"/>
     </row>
-    <row r="5" spans="1:21" s="1" customFormat="1" ht="128" customHeight="1" thickBot="1">
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="128" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -3516,7 +3498,7 @@
       <c r="T5" s="53"/>
       <c r="U5" s="53"/>
     </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" ht="23" thickBot="1">
+    <row r="6" spans="1:21" s="3" customFormat="1" ht="23" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
         <v>0</v>
       </c>
@@ -3557,8 +3539,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="45" thickBot="1">
-      <c r="A7" s="11"/>
+    <row r="7" spans="1:21" ht="45" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>147</v>
+      </c>
       <c r="B7" s="65" t="s">
         <v>81</v>
       </c>
@@ -3597,8 +3581,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="56" thickBot="1">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:21" ht="56" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>148</v>
+      </c>
       <c r="B8" s="65" t="s">
         <v>8</v>
       </c>
@@ -3636,8 +3622,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="34" thickBot="1">
-      <c r="A9" s="11"/>
+    <row r="9" spans="1:21" ht="34" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>149</v>
+      </c>
       <c r="B9" s="65" t="s">
         <v>8</v>
       </c>
@@ -3676,8 +3664,10 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="45" thickBot="1">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:21" ht="45" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>150</v>
+      </c>
       <c r="B10" s="65" t="s">
         <v>81</v>
       </c>
@@ -3716,8 +3706,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="46" customHeight="1" thickBot="1">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:21" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>151</v>
+      </c>
       <c r="B11" s="65" t="s">
         <v>8</v>
       </c>
@@ -3752,8 +3744,10 @@
       </c>
       <c r="M11" s="93"/>
     </row>
-    <row r="12" spans="1:21" ht="45" thickBot="1">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:21" ht="45" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>152</v>
+      </c>
       <c r="B12" s="65" t="s">
         <v>81</v>
       </c>
@@ -3792,8 +3786,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="45" thickBot="1">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:21" ht="45" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="B13" s="65" t="s">
         <v>81</v>
       </c>
@@ -3808,32 +3804,34 @@
         <v>Closed</v>
       </c>
       <c r="F13" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="68" t="s">
+      <c r="H13" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" s="97" t="s">
         <v>124</v>
       </c>
-      <c r="H13" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="I13" s="97" t="s">
-        <v>125</v>
-      </c>
       <c r="J13" s="93" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="K13" s="70" t="s">
         <v>68</v>
       </c>
       <c r="L13" s="64" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="M13" s="93" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="34" thickBot="1">
-      <c r="A14" s="12"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="34" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>154</v>
+      </c>
       <c r="B14" s="65" t="s">
         <v>81</v>
       </c>
@@ -3848,32 +3846,34 @@
         <v>Closed</v>
       </c>
       <c r="F14" s="74" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="G14" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H14" s="68" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I14" s="97" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J14" s="93" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="K14" s="70" t="s">
         <v>68</v>
       </c>
       <c r="L14" s="64" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="M14" s="93" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="45" thickBot="1">
-      <c r="A15" s="12"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="45" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="B15" s="65" t="s">
         <v>81</v>
       </c>
@@ -3888,32 +3888,34 @@
         <v>Closed</v>
       </c>
       <c r="F15" s="74" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G15" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" s="68" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I15" s="97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J15" s="93" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="K15" s="70" t="s">
         <v>68</v>
       </c>
       <c r="L15" s="64" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="M15" s="93" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="34" thickBot="1">
-      <c r="A16" s="12"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="34" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="B16" s="65" t="s">
         <v>81</v>
       </c>
@@ -3928,32 +3930,34 @@
         <v>Closed</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G16" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H16" s="68" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I16" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="93" t="s">
         <v>140</v>
-      </c>
-      <c r="J16" s="93" t="s">
-        <v>128</v>
       </c>
       <c r="K16" s="70" t="s">
         <v>68</v>
       </c>
       <c r="L16" s="64" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="M16" s="93" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="34" thickBot="1">
-      <c r="A17" s="12"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="34" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>157</v>
+      </c>
       <c r="B17" s="65" t="s">
         <v>81</v>
       </c>
@@ -3968,32 +3972,34 @@
         <v>Closed</v>
       </c>
       <c r="F17" s="74" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G17" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H17" s="68" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I17" s="97" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="J17" s="93" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="K17" s="70" t="s">
         <v>68</v>
       </c>
       <c r="L17" s="64" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="M17" s="93" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="34" thickBot="1">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:13" ht="34" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="B18" s="65" t="s">
         <v>8</v>
       </c>
@@ -4008,27 +4014,31 @@
         <v>Yellow</v>
       </c>
       <c r="F18" s="74" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G18" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H18" s="68" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I18" s="97" t="s">
-        <v>132</v>
-      </c>
-      <c r="J18" s="93"/>
+        <v>159</v>
+      </c>
+      <c r="J18" s="93" t="s">
+        <v>160</v>
+      </c>
       <c r="K18" s="95" t="s">
         <v>90</v>
       </c>
       <c r="L18" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="M18" s="93"/>
-    </row>
-    <row r="19" spans="1:13">
+        <v>127</v>
+      </c>
+      <c r="M18" s="93" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="12"/>
       <c r="B19" s="14"/>
       <c r="C19" s="27"/>
@@ -4046,7 +4056,7 @@
       <c r="L19" s="14"/>
       <c r="M19" s="34"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="12"/>
       <c r="B20" s="14"/>
       <c r="C20" s="27"/>
@@ -4064,7 +4074,7 @@
       <c r="L20" s="60"/>
       <c r="M20" s="34"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" s="12"/>
       <c r="B21" s="14"/>
       <c r="C21" s="27"/>
@@ -4082,7 +4092,7 @@
       <c r="L21" s="60"/>
       <c r="M21" s="34"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="12"/>
       <c r="B22" s="14"/>
       <c r="C22" s="27"/>
@@ -4100,7 +4110,7 @@
       <c r="L22" s="60"/>
       <c r="M22" s="34"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="12"/>
       <c r="B23" s="14"/>
       <c r="C23" s="27"/>
@@ -4118,7 +4128,7 @@
       <c r="L23" s="60"/>
       <c r="M23" s="34"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
       <c r="C24" s="27"/>
@@ -4136,7 +4146,7 @@
       <c r="L24" s="60"/>
       <c r="M24" s="34"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="12"/>
       <c r="B25" s="14"/>
       <c r="C25" s="27"/>
@@ -4154,7 +4164,7 @@
       <c r="L25" s="60"/>
       <c r="M25" s="34"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="12"/>
       <c r="B26" s="14"/>
       <c r="C26" s="27"/>
@@ -4172,7 +4182,7 @@
       <c r="L26" s="60"/>
       <c r="M26" s="34"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="12"/>
       <c r="B27" s="14"/>
       <c r="C27" s="27"/>
@@ -4190,7 +4200,7 @@
       <c r="L27" s="60"/>
       <c r="M27" s="34"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="12"/>
       <c r="B28" s="14"/>
       <c r="C28" s="27"/>
@@ -4208,7 +4218,7 @@
       <c r="L28" s="60"/>
       <c r="M28" s="34"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="12"/>
       <c r="B29" s="14"/>
       <c r="C29" s="27"/>
@@ -4226,7 +4236,7 @@
       <c r="L29" s="60"/>
       <c r="M29" s="34"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="12"/>
       <c r="B30" s="14"/>
       <c r="C30" s="27"/>
@@ -4244,7 +4254,7 @@
       <c r="L30" s="60"/>
       <c r="M30" s="34"/>
     </row>
-    <row r="31" spans="1:13" ht="14" thickBot="1">
+    <row r="31" spans="1:13" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="14"/>
       <c r="C31" s="27"/>
@@ -4262,7 +4272,7 @@
       <c r="L31" s="60"/>
       <c r="M31" s="34"/>
     </row>
-    <row r="32" spans="1:13" ht="14" thickBot="1">
+    <row r="32" spans="1:13" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="15"/>
       <c r="C32" s="48"/>
@@ -4283,175 +4293,175 @@
   <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C33:E65533 C1:E1 B6:C6 B7:B12 B19:B32">
-    <cfRule type="cellIs" dxfId="73" priority="64" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="64" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="65" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="65" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="66" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19:L32">
-    <cfRule type="cellIs" dxfId="70" priority="67" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="67" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="68" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E12 E19:E32">
-    <cfRule type="cellIs" dxfId="68" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="69" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="70" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="71" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="71" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D12 C19:D32">
-    <cfRule type="cellIs" dxfId="65" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="72" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="73" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="74" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="74" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="62" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="55" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="56" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="57" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="59" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="59" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:D13">
-    <cfRule type="cellIs" dxfId="56" priority="61" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="61" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="62" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="63" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="63" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="53" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="47" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="48" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="50" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="49" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="50" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="51" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:D14">
-    <cfRule type="cellIs" dxfId="47" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="52" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="54" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="44" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="38" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="41" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:D15">
-    <cfRule type="cellIs" dxfId="38" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="43" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="45" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="35" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="32" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:D16">
-    <cfRule type="cellIs" dxfId="29" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="34" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4552,107 +4562,107 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14" thickBot="1">
+    <row r="1" spans="1:1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="46" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" s="46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="46" t="s">
         <v>44</v>
       </c>

</xml_diff>